<commit_message>
feat: add data sample
</commit_message>
<xml_diff>
--- a/data_sample/AU/lucymarieslatter@gmail.com/Inventory Age - lucymarieslatter@gmail.com.xlsx
+++ b/data_sample/AU/lucymarieslatter@gmail.com/Inventory Age - lucymarieslatter@gmail.com.xlsx
@@ -1620,23 +1620,29 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Tài liệu" ma:contentTypeID="0x0101008448199DFACA154686D82DCDC168157D" ma:contentTypeVersion="8" ma:contentTypeDescription="Tạo tài liệu mới." ma:contentTypeScope="" ma:versionID="70aae43183516f193a389d50d6008a34">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5447f5c2-7fc2-4801-bece-2e3a488b5462" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f9155bdd6865efe30c75a4f2e4789de" ns2:_="">
-    <xsd:import namespace="5447f5c2-7fc2-4801-bece-2e3a488b5462"/>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BBBFDDD24E42164EAFB1232386063B6A" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4b1c95c0cec284925124a8213c49e4d8">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9349b505-b62a-4b43-a195-82e3366bf674" xmlns:ns3="e4ad1741-f329-4dc2-b2ab-bf833ccef93b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d8f563a9d69e5946b7f0bb5c4c106df6" ns2:_="" ns3:_="">
+    <xsd:import namespace="9349b505-b62a-4b43-a195-82e3366bf674"/>
+    <xsd:import namespace="e4ad1741-f329-4dc2-b2ab-bf833ccef93b"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element name="documentManagement">
             <xsd:complexType>
               <xsd:all>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns2:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -1644,45 +1650,94 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="5447f5c2-7fc2-4801-bece-2e3a488b5462" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="9349b505-b62a-4b43-a195-82e3366bf674" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="8" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="9" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="e4ad1741-f329-4dc2-b2ab-bf833ccef93b" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="10" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+    <xsd:element name="MediaServiceFastMetadata" ma:index="11" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+    <xsd:element name="MediaServiceDateTaken" ma:index="12" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="13" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="11" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+    <xsd:element name="MediaServiceKeyPoints" ma:index="14" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="15" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="12" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+    <xsd:element name="MediaServiceOCR" ma:index="16" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="13" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+    <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="14" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+    <xsd:element name="MediaServiceLocation" ma:index="19" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="15" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+    <xsd:element name="MediaLengthInSeconds" ma:index="20" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
@@ -1697,8 +1752,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Loại Nội dung"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Tiêu đề"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -1789,9 +1844,7 @@
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MediaLengthInSeconds xmlns="5447f5c2-7fc2-4801-bece-2e3a488b5462" xsi:nil="true"/>
-  </documentManagement>
+  <documentManagement/>
 </p:properties>
 </file>
 
@@ -1805,7 +1858,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7293906D-EDFA-443D-9703-89B8FC47518E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECB8FBA3-E7AB-4463-9F21-07C312BF0BA5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9349b505-b62a-4b43-a195-82e3366bf674"/>
+    <ds:schemaRef ds:uri="e4ad1741-f329-4dc2-b2ab-bf833ccef93b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>